<commit_message>
feat: added edit user in Bio, refactored logs to accomodate modularity
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C248"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,7 +421,7 @@
         <v>RODEL</v>
       </c>
       <c r="C2" t="str">
-        <v>Mon Oct 07 2024 08:29:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:01:09</v>
       </c>
     </row>
     <row r="3">
@@ -432,7 +432,7 @@
         <v>RODEL</v>
       </c>
       <c r="C3" t="str">
-        <v>Mon Oct 07 2024 17:06:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 18:04:31</v>
       </c>
     </row>
     <row r="4">
@@ -443,7 +443,7 @@
         <v>RODEL</v>
       </c>
       <c r="C4" t="str">
-        <v>Tue Oct 08 2024 07:20:12 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:32:06</v>
       </c>
     </row>
     <row r="5">
@@ -454,7 +454,7 @@
         <v>RODEL</v>
       </c>
       <c r="C5" t="str">
-        <v>Tue Oct 08 2024 17:07:02 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:03:26</v>
       </c>
     </row>
     <row r="6">
@@ -465,7 +465,7 @@
         <v>RODEL</v>
       </c>
       <c r="C6" t="str">
-        <v>Wed Oct 09 2024 07:01:09 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:37:40</v>
       </c>
     </row>
     <row r="7">
@@ -476,7 +476,7 @@
         <v>RODEL</v>
       </c>
       <c r="C7" t="str">
-        <v>Wed Oct 09 2024 18:04:31 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 17:17:56</v>
       </c>
     </row>
     <row r="8">
@@ -487,7 +487,7 @@
         <v>RODEL</v>
       </c>
       <c r="C8" t="str">
-        <v>Thu Oct 10 2024 07:32:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 08:32:11</v>
       </c>
     </row>
     <row r="9">
@@ -498,7 +498,7 @@
         <v>RODEL</v>
       </c>
       <c r="C9" t="str">
-        <v>Thu Oct 10 2024 14:31:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 08:40:03</v>
       </c>
     </row>
     <row r="10">
@@ -509,7 +509,7 @@
         <v>DEL</v>
       </c>
       <c r="C10" t="str">
-        <v>Mon Oct 07 2024 09:06:52 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 08:47:19</v>
       </c>
     </row>
     <row r="11">
@@ -520,7 +520,7 @@
         <v>DEL</v>
       </c>
       <c r="C11" t="str">
-        <v>Mon Oct 07 2024 18:02:30 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 18:03:59</v>
       </c>
     </row>
     <row r="12">
@@ -531,7 +531,7 @@
         <v>DEL</v>
       </c>
       <c r="C12" t="str">
-        <v>Tue Oct 08 2024 10:37:32 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 08:50:15</v>
       </c>
     </row>
     <row r="13">
@@ -542,7 +542,7 @@
         <v>DEL</v>
       </c>
       <c r="C13" t="str">
-        <v>Tue Oct 08 2024 18:00:59 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:19:36</v>
       </c>
     </row>
     <row r="14">
@@ -553,7 +553,7 @@
         <v>DEL</v>
       </c>
       <c r="C14" t="str">
-        <v>Wed Oct 09 2024 08:47:19 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 09:08:12</v>
       </c>
     </row>
     <row r="15">
@@ -564,62 +564,62 @@
         <v>DEL</v>
       </c>
       <c r="C15" t="str">
-        <v>Wed Oct 09 2024 18:03:59 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 18:10:19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>1011</v>
+        <v>902</v>
       </c>
       <c r="B16" t="str">
-        <v>DEL</v>
+        <v>ANDY</v>
       </c>
       <c r="C16" t="str">
-        <v>Thu Oct 10 2024 08:50:15 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 14:03:52</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>1011</v>
+        <v>5001</v>
       </c>
       <c r="B17" t="str">
-        <v>DEL</v>
+        <v>CRISTINE</v>
       </c>
       <c r="C17" t="str">
-        <v>Thu Oct 10 2024 15:10:25 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 09:12:02</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>902</v>
+        <v>5001</v>
       </c>
       <c r="B18" t="str">
-        <v>ANDY</v>
+        <v>CRISTINE</v>
       </c>
       <c r="C18" t="str">
-        <v>Mon Oct 07 2024 16:52:19 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:41:13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>1019</v>
+        <v>5001</v>
       </c>
       <c r="B19" t="str">
-        <v>DENNIS</v>
+        <v>CRISTINE</v>
       </c>
       <c r="C19" t="str">
-        <v>Mon Oct 07 2024 10:30:47 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 08:38:38</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>1019</v>
+        <v>5001</v>
       </c>
       <c r="B20" t="str">
-        <v>DENNIS</v>
+        <v>CRISTINE</v>
       </c>
       <c r="C20" t="str">
-        <v>Mon Oct 07 2024 11:34:33 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 20:40:46</v>
       </c>
     </row>
     <row r="21">
@@ -630,7 +630,7 @@
         <v>CRISTINE</v>
       </c>
       <c r="C21" t="str">
-        <v>Mon Oct 07 2024 09:01:12 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 08:48:32</v>
       </c>
     </row>
     <row r="22">
@@ -641,139 +641,139 @@
         <v>CRISTINE</v>
       </c>
       <c r="C22" t="str">
-        <v>Mon Oct 07 2024 18:14:31 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 19:43:55</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>5001</v>
+        <v>4015</v>
       </c>
       <c r="B23" t="str">
-        <v>CRISTINE</v>
+        <v>AKEYLA</v>
       </c>
       <c r="C23" t="str">
-        <v>Tue Oct 08 2024 08:50:27 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 09:54:00</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>5001</v>
+        <v>4015</v>
       </c>
       <c r="B24" t="str">
-        <v>CRISTINE</v>
+        <v>AKEYLA</v>
       </c>
       <c r="C24" t="str">
-        <v>Tue Oct 08 2024 18:08:03 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:59:59</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>5001</v>
+        <v>4015</v>
       </c>
       <c r="B25" t="str">
-        <v>CRISTINE</v>
+        <v>AKEYLA</v>
       </c>
       <c r="C25" t="str">
-        <v>Wed Oct 09 2024 09:12:02 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 09:48:13</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>5001</v>
+        <v>4015</v>
       </c>
       <c r="B26" t="str">
-        <v>CRISTINE</v>
+        <v>AKEYLA</v>
       </c>
       <c r="C26" t="str">
-        <v>Wed Oct 09 2024 17:41:13 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 18:59:32</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>5001</v>
+        <v>4015</v>
       </c>
       <c r="B27" t="str">
-        <v>CRISTINE</v>
+        <v>AKEYLA</v>
       </c>
       <c r="C27" t="str">
-        <v>Thu Oct 10 2024 08:38:38 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 09:45:46</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>5001</v>
+        <v>4015</v>
       </c>
       <c r="B28" t="str">
-        <v>CRISTINE</v>
+        <v>AKEYLA</v>
       </c>
       <c r="C28" t="str">
-        <v>Thu Oct 10 2024 15:19:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 18:00:49</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>4015</v>
+        <v>908</v>
       </c>
       <c r="B29" t="str">
-        <v>AKEYLA</v>
+        <v>LEO</v>
       </c>
       <c r="C29" t="str">
-        <v>Tue Oct 08 2024 09:33:30 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:54:23</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>4015</v>
+        <v>908</v>
       </c>
       <c r="B30" t="str">
-        <v>AKEYLA</v>
+        <v>LEO</v>
       </c>
       <c r="C30" t="str">
-        <v>Tue Oct 08 2024 18:01:03 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 18:03:34</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>4015</v>
+        <v>908</v>
       </c>
       <c r="B31" t="str">
-        <v>AKEYLA</v>
+        <v>LEO</v>
       </c>
       <c r="C31" t="str">
-        <v>Wed Oct 09 2024 09:54:00 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 13:58:23</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>4015</v>
+        <v>908</v>
       </c>
       <c r="B32" t="str">
-        <v>AKEYLA</v>
+        <v>LEO</v>
       </c>
       <c r="C32" t="str">
-        <v>Wed Oct 09 2024 17:59:59 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 16:17:15</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>4015</v>
+        <v>908</v>
       </c>
       <c r="B33" t="str">
-        <v>AKEYLA</v>
+        <v>LEO</v>
       </c>
       <c r="C33" t="str">
-        <v>Thu Oct 10 2024 09:48:13 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 18:07:38</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>4015</v>
+        <v>908</v>
       </c>
       <c r="B34" t="str">
-        <v>AKEYLA</v>
+        <v>LEO</v>
       </c>
       <c r="C34" t="str">
-        <v>Thu Oct 10 2024 14:08:17 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-13 07:54:37</v>
       </c>
     </row>
     <row r="35">
@@ -784,7 +784,7 @@
         <v>LEO</v>
       </c>
       <c r="C35" t="str">
-        <v>Wed Oct 09 2024 07:54:23 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-13 18:03:44</v>
       </c>
     </row>
     <row r="36">
@@ -795,18 +795,18 @@
         <v>LEO</v>
       </c>
       <c r="C36" t="str">
-        <v>Wed Oct 09 2024 18:03:34 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:56:00</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>908</v>
+        <v>5003</v>
       </c>
       <c r="B37" t="str">
-        <v>LEO</v>
+        <v>FRANCIS</v>
       </c>
       <c r="C37" t="str">
-        <v>Thu Oct 10 2024 13:58:23 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 09:53:06</v>
       </c>
     </row>
     <row r="38">
@@ -817,7 +817,7 @@
         <v>FRANCIS</v>
       </c>
       <c r="C38" t="str">
-        <v>Mon Oct 07 2024 09:47:40 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 13:52:04</v>
       </c>
     </row>
     <row r="39">
@@ -828,51 +828,51 @@
         <v>FRANCIS</v>
       </c>
       <c r="C39" t="str">
-        <v>Mon Oct 07 2024 14:33:09 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 13:50:51</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>5003</v>
+        <v>5005</v>
       </c>
       <c r="B40" t="str">
-        <v>FRANCIS</v>
+        <v>ERIKA</v>
       </c>
       <c r="C40" t="str">
-        <v>Tue Oct 08 2024 10:12:30 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 10:03:27</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>5003</v>
+        <v>5005</v>
       </c>
       <c r="B41" t="str">
-        <v>FRANCIS</v>
+        <v>ERIKA</v>
       </c>
       <c r="C41" t="str">
-        <v>Tue Oct 08 2024 18:51:40 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 18:52:29</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>5003</v>
+        <v>5005</v>
       </c>
       <c r="B42" t="str">
-        <v>FRANCIS</v>
+        <v>ERIKA</v>
       </c>
       <c r="C42" t="str">
-        <v>Wed Oct 09 2024 09:53:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 09:26:32</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>5003</v>
+        <v>5005</v>
       </c>
       <c r="B43" t="str">
-        <v>FRANCIS</v>
+        <v>ERIKA</v>
       </c>
       <c r="C43" t="str">
-        <v>Wed Oct 09 2024 13:52:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 14:37:54</v>
       </c>
     </row>
     <row r="44">
@@ -883,7 +883,7 @@
         <v>ERIKA</v>
       </c>
       <c r="C44" t="str">
-        <v>Mon Oct 07 2024 09:51:16 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 13:16:49</v>
       </c>
     </row>
     <row r="45">
@@ -894,2245 +894,1882 @@
         <v>ERIKA</v>
       </c>
       <c r="C45" t="str">
-        <v>Mon Oct 07 2024 18:54:40 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 19:00:02</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>5005</v>
+        <v>5006</v>
       </c>
       <c r="B46" t="str">
-        <v>ERIKA</v>
+        <v>DENNY</v>
       </c>
       <c r="C46" t="str">
-        <v>Tue Oct 08 2024 14:52:31 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:28:41</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>5005</v>
+        <v>5006</v>
       </c>
       <c r="B47" t="str">
-        <v>ERIKA</v>
+        <v>DENNY</v>
       </c>
       <c r="C47" t="str">
-        <v>Tue Oct 08 2024 17:37:56 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 12:50:04</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>5005</v>
+        <v>5006</v>
       </c>
       <c r="B48" t="str">
-        <v>ERIKA</v>
+        <v>DENNY</v>
       </c>
       <c r="C48" t="str">
-        <v>Wed Oct 09 2024 10:03:27 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 10:55:35</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>5005</v>
+        <v>5006</v>
       </c>
       <c r="B49" t="str">
-        <v>ERIKA</v>
+        <v>DENNY</v>
       </c>
       <c r="C49" t="str">
-        <v>Wed Oct 09 2024 18:52:29 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 16:11:02</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>5005</v>
+        <v>5006</v>
       </c>
       <c r="B50" t="str">
-        <v>ERIKA</v>
+        <v>DENNY</v>
       </c>
       <c r="C50" t="str">
-        <v>Thu Oct 10 2024 09:26:32 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:36:27</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>5005</v>
+        <v>5006</v>
       </c>
       <c r="B51" t="str">
-        <v>ERIKA</v>
+        <v>DENNY</v>
       </c>
       <c r="C51" t="str">
-        <v>Thu Oct 10 2024 14:37:54 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:36:30</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>5006</v>
+        <v>5007</v>
       </c>
       <c r="B52" t="str">
-        <v>DENNY</v>
+        <v>PAUL</v>
       </c>
       <c r="C52" t="str">
-        <v>Mon Oct 07 2024 07:56:49 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 16:45:16</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>5006</v>
+        <v>5008</v>
       </c>
       <c r="B53" t="str">
-        <v>DENNY</v>
+        <v>MILES</v>
       </c>
       <c r="C53" t="str">
-        <v>Mon Oct 07 2024 15:00:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:34:28</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>5006</v>
+        <v>5008</v>
       </c>
       <c r="B54" t="str">
-        <v>DENNY</v>
+        <v>MILES</v>
       </c>
       <c r="C54" t="str">
-        <v>Tue Oct 08 2024 07:48:39 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:01:49</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>5006</v>
+        <v>5008</v>
       </c>
       <c r="B55" t="str">
-        <v>DENNY</v>
+        <v>MILES</v>
       </c>
       <c r="C55" t="str">
-        <v>Tue Oct 08 2024 17:04:34 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:58:14</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>5006</v>
+        <v>5008</v>
       </c>
       <c r="B56" t="str">
-        <v>DENNY</v>
+        <v>MILES</v>
       </c>
       <c r="C56" t="str">
-        <v>Wed Oct 09 2024 07:28:41 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:02:19</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>5006</v>
+        <v>5008</v>
       </c>
       <c r="B57" t="str">
-        <v>DENNY</v>
+        <v>MILES</v>
       </c>
       <c r="C57" t="str">
-        <v>Wed Oct 09 2024 12:50:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:21:50</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>5006</v>
+        <v>5008</v>
       </c>
       <c r="B58" t="str">
-        <v>DENNY</v>
+        <v>MILES</v>
       </c>
       <c r="C58" t="str">
-        <v>Thu Oct 10 2024 10:55:35 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 08:02:49</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>5006</v>
+        <v>4011</v>
       </c>
       <c r="B59" t="str">
-        <v>DENNY</v>
+        <v>ANDY RUSSEL</v>
       </c>
       <c r="C59" t="str">
-        <v>Thu Oct 10 2024 14:13:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:36:10</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>5007</v>
+        <v>4011</v>
       </c>
       <c r="B60" t="str">
-        <v>PAUL</v>
+        <v>ANDY RUSSEL</v>
       </c>
       <c r="C60" t="str">
-        <v>Mon Oct 07 2024 10:19:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 13:17:20</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>5007</v>
+        <v>4011</v>
       </c>
       <c r="B61" t="str">
-        <v>PAUL</v>
+        <v>ANDY RUSSEL</v>
       </c>
       <c r="C61" t="str">
-        <v>Mon Oct 07 2024 17:35:47 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 11:21:14</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>5008</v>
+        <v>4011</v>
       </c>
       <c r="B62" t="str">
-        <v>MILES</v>
+        <v>ANDY RUSSEL</v>
       </c>
       <c r="C62" t="str">
-        <v>Mon Oct 07 2024 07:25:50 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 14:59:19</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>5008</v>
+        <v>4011</v>
       </c>
       <c r="B63" t="str">
-        <v>MILES</v>
+        <v>ANDY RUSSEL</v>
       </c>
       <c r="C63" t="str">
-        <v>Mon Oct 07 2024 17:01:41 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 10:46:23</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>5008</v>
+        <v>4011</v>
       </c>
       <c r="B64" t="str">
-        <v>MILES</v>
+        <v>ANDY RUSSEL</v>
       </c>
       <c r="C64" t="str">
-        <v>Tue Oct 08 2024 07:59:23 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 16:57:07</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>5008</v>
+        <v>4011</v>
       </c>
       <c r="B65" t="str">
-        <v>MILES</v>
+        <v>ANDY RUSSEL</v>
       </c>
       <c r="C65" t="str">
-        <v>Tue Oct 08 2024 17:02:47 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:58:11</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>5008</v>
+        <v>4008</v>
       </c>
       <c r="B66" t="str">
-        <v>MILES</v>
+        <v>MAECHELLE</v>
       </c>
       <c r="C66" t="str">
-        <v>Wed Oct 09 2024 07:34:28 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:46:17</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>5008</v>
+        <v>4008</v>
       </c>
       <c r="B67" t="str">
-        <v>MILES</v>
+        <v>MAECHELLE</v>
       </c>
       <c r="C67" t="str">
-        <v>Wed Oct 09 2024 17:01:49 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 10:29:37</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>5008</v>
+        <v>4008</v>
       </c>
       <c r="B68" t="str">
-        <v>MILES</v>
+        <v>MAECHELLE</v>
       </c>
       <c r="C68" t="str">
-        <v>Thu Oct 10 2024 07:58:14 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 16:17:31</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>5008</v>
+        <v>4008</v>
       </c>
       <c r="B69" t="str">
-        <v>MILES</v>
+        <v>MAECHELLE</v>
       </c>
       <c r="C69" t="str">
-        <v>Thu Oct 10 2024 13:33:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 16:17:34</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>4011</v>
+        <v>4008</v>
       </c>
       <c r="B70" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>MAECHELLE</v>
       </c>
       <c r="C70" t="str">
-        <v>Mon Oct 07 2024 10:16:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 13:15:46</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>4011</v>
+        <v>4008</v>
       </c>
       <c r="B71" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>MAECHELLE</v>
       </c>
       <c r="C71" t="str">
-        <v>Mon Oct 07 2024 16:42:52 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 13:34:51</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>4011</v>
+        <v>4008</v>
       </c>
       <c r="B72" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>MAECHELLE</v>
       </c>
       <c r="C72" t="str">
-        <v>Tue Oct 08 2024 12:07:51 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:48:47</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>4011</v>
+        <v>4009</v>
       </c>
       <c r="B73" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>HUBERT LOPEZ</v>
       </c>
       <c r="C73" t="str">
-        <v>Tue Oct 08 2024 13:11:52 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 13:05:33</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>4011</v>
+        <v>4009</v>
       </c>
       <c r="B74" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>HUBERT LOPEZ</v>
       </c>
       <c r="C74" t="str">
-        <v>Wed Oct 09 2024 07:36:10 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 19:07:44</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>4011</v>
+        <v>4009</v>
       </c>
       <c r="B75" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>HUBERT LOPEZ</v>
       </c>
       <c r="C75" t="str">
-        <v>Wed Oct 09 2024 13:17:20 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 18:51:01</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>4011</v>
+        <v>4009</v>
       </c>
       <c r="B76" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>HUBERT LOPEZ</v>
       </c>
       <c r="C76" t="str">
-        <v>Thu Oct 10 2024 11:21:14 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 18:55:04</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>4011</v>
+        <v>5010</v>
       </c>
       <c r="B77" t="str">
-        <v>ANDY RUSSEL</v>
+        <v>CORTEJO</v>
       </c>
       <c r="C77" t="str">
-        <v>Thu Oct 10 2024 14:59:19 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 06:57:26</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>4008</v>
+        <v>5010</v>
       </c>
       <c r="B78" t="str">
-        <v>MAECHELLE</v>
+        <v>CORTEJO</v>
       </c>
       <c r="C78" t="str">
-        <v>Mon Oct 07 2024 07:41:46 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:06:56</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>4008</v>
+        <v>5010</v>
       </c>
       <c r="B79" t="str">
-        <v>MAECHELLE</v>
+        <v>CORTEJO</v>
       </c>
       <c r="C79" t="str">
-        <v>Mon Oct 07 2024 16:58:49 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 06:49:09</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>4008</v>
+        <v>5010</v>
       </c>
       <c r="B80" t="str">
-        <v>MAECHELLE</v>
+        <v>CORTEJO</v>
       </c>
       <c r="C80" t="str">
-        <v>Tue Oct 08 2024 07:45:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:00:05</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>4008</v>
+        <v>5010</v>
       </c>
       <c r="B81" t="str">
-        <v>MAECHELLE</v>
+        <v>CORTEJO</v>
       </c>
       <c r="C81" t="str">
-        <v>Tue Oct 08 2024 14:58:57 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 06:43:03</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>4008</v>
+        <v>5010</v>
       </c>
       <c r="B82" t="str">
-        <v>MAECHELLE</v>
+        <v>CORTEJO</v>
       </c>
       <c r="C82" t="str">
-        <v>Wed Oct 09 2024 07:46:17 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 17:00:48</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>4008</v>
+        <v>5010</v>
       </c>
       <c r="B83" t="str">
-        <v>MAECHELLE</v>
+        <v>CORTEJO</v>
       </c>
       <c r="C83" t="str">
-        <v>Wed Oct 09 2024 10:29:37 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 06:50:42</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>4009</v>
+        <v>5011</v>
       </c>
       <c r="B84" t="str">
-        <v>HUBERT LOPEZ</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C84" t="str">
-        <v>Mon Oct 07 2024 15:49:40 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 12:18:31</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>4009</v>
+        <v>5011</v>
       </c>
       <c r="B85" t="str">
-        <v>HUBERT LOPEZ</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C85" t="str">
-        <v>Mon Oct 07 2024 18:21:51 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:06:59</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>4009</v>
+        <v>5011</v>
       </c>
       <c r="B86" t="str">
-        <v>HUBERT LOPEZ</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C86" t="str">
-        <v>Tue Oct 08 2024 11:27:38 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 06:43:39</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>4009</v>
+        <v>5011</v>
       </c>
       <c r="B87" t="str">
-        <v>HUBERT LOPEZ</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C87" t="str">
-        <v>Tue Oct 08 2024 18:07:21 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:00:20</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>4009</v>
+        <v>5011</v>
       </c>
       <c r="B88" t="str">
-        <v>HUBERT LOPEZ</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C88" t="str">
-        <v>Thu Oct 10 2024 13:05:33 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:16:24</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>5010</v>
+        <v>5011</v>
       </c>
       <c r="B89" t="str">
-        <v>CORTEJO</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C89" t="str">
-        <v>Mon Oct 07 2024 07:08:37 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 17:00:54</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>5010</v>
+        <v>5011</v>
       </c>
       <c r="B90" t="str">
-        <v>CORTEJO</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C90" t="str">
-        <v>Mon Oct 07 2024 17:00:52 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:12:32</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>5010</v>
+        <v>5011</v>
       </c>
       <c r="B91" t="str">
-        <v>CORTEJO</v>
+        <v>VINCENT TAN</v>
       </c>
       <c r="C91" t="str">
-        <v>Tue Oct 08 2024 06:45:42 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:56:46</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>5010</v>
+        <v>1025</v>
       </c>
       <c r="B92" t="str">
-        <v>CORTEJO</v>
+        <v>Lyndon</v>
       </c>
       <c r="C92" t="str">
-        <v>Tue Oct 08 2024 17:00:14 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 08:00:10</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>5010</v>
+        <v>1025</v>
       </c>
       <c r="B93" t="str">
-        <v>CORTEJO</v>
+        <v>Lyndon</v>
       </c>
       <c r="C93" t="str">
-        <v>Wed Oct 09 2024 06:57:26 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 14:39:04</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>5010</v>
+        <v>1025</v>
       </c>
       <c r="B94" t="str">
-        <v>CORTEJO</v>
+        <v>Lyndon</v>
       </c>
       <c r="C94" t="str">
-        <v>Wed Oct 09 2024 17:06:56 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:28:36</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>5010</v>
+        <v>1025</v>
       </c>
       <c r="B95" t="str">
-        <v>CORTEJO</v>
+        <v>Lyndon</v>
       </c>
       <c r="C95" t="str">
-        <v>Thu Oct 10 2024 06:49:09 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 15:56:51</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>5010</v>
+        <v>1025</v>
       </c>
       <c r="B96" t="str">
-        <v>CORTEJO</v>
+        <v>Lyndon</v>
       </c>
       <c r="C96" t="str">
-        <v>Thu Oct 10 2024 07:16:46 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 08:08:02</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>5011</v>
+        <v>1025</v>
       </c>
       <c r="B97" t="str">
-        <v>VINCENT</v>
+        <v>Lyndon</v>
       </c>
       <c r="C97" t="str">
-        <v>Mon Oct 07 2024 07:07:18 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 15:19:30</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>5011</v>
+        <v>1025</v>
       </c>
       <c r="B98" t="str">
-        <v>VINCENT</v>
+        <v>Lyndon</v>
       </c>
       <c r="C98" t="str">
-        <v>Mon Oct 07 2024 17:01:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:47:25</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>5011</v>
+        <v>1027</v>
       </c>
       <c r="B99" t="str">
-        <v>VINCENT</v>
+        <v>Lordemil</v>
       </c>
       <c r="C99" t="str">
-        <v>Tue Oct 08 2024 07:00:38 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 12:20:46</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>5011</v>
+        <v>1027</v>
       </c>
       <c r="B100" t="str">
-        <v>VINCENT</v>
+        <v>Lordemil</v>
       </c>
       <c r="C100" t="str">
-        <v>Tue Oct 08 2024 17:03:13 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 19:07:41</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>5011</v>
+        <v>1027</v>
       </c>
       <c r="B101" t="str">
-        <v>VINCENT</v>
+        <v>Lordemil</v>
       </c>
       <c r="C101" t="str">
-        <v>Wed Oct 09 2024 12:18:31 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 12:45:38</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>5011</v>
+        <v>1027</v>
       </c>
       <c r="B102" t="str">
-        <v>VINCENT</v>
+        <v>Lordemil</v>
       </c>
       <c r="C102" t="str">
-        <v>Wed Oct 09 2024 17:06:59 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 14:37:22</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>5011</v>
+        <v>1027</v>
       </c>
       <c r="B103" t="str">
-        <v>VINCENT</v>
+        <v>Lordemil</v>
       </c>
       <c r="C103" t="str">
-        <v>Thu Oct 10 2024 06:43:39 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 11:52:05</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>5011</v>
+        <v>1027</v>
       </c>
       <c r="B104" t="str">
-        <v>VINCENT</v>
+        <v>Lordemil</v>
       </c>
       <c r="C104" t="str">
-        <v>Thu Oct 10 2024 14:28:13 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 21:00:58</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B105" t="str">
-        <v>Lyndon</v>
+        <v>Jane</v>
       </c>
       <c r="C105" t="str">
-        <v>Wed Oct 09 2024 08:00:10 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:42:16</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B106" t="str">
-        <v>Lyndon</v>
+        <v>Jane</v>
       </c>
       <c r="C106" t="str">
-        <v>Wed Oct 09 2024 14:39:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 15:28:39</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B107" t="str">
-        <v>Lyndon</v>
+        <v>Jane</v>
       </c>
       <c r="C107" t="str">
-        <v>Thu Oct 10 2024 07:28:36 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:59:19</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B108" t="str">
-        <v>Lyndon</v>
+        <v>Jane</v>
       </c>
       <c r="C108" t="str">
-        <v>Thu Oct 10 2024 14:47:48 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 14:31:09</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="B109" t="str">
-        <v>Lordemil</v>
+        <v>Jane</v>
       </c>
       <c r="C109" t="str">
-        <v>Mon Oct 07 2024 14:05:38 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:41:16</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="B110" t="str">
-        <v>Lordemil</v>
+        <v>Jane</v>
       </c>
       <c r="C110" t="str">
-        <v>Mon Oct 07 2024 19:18:48 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 08:37:01</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>1027</v>
+        <v>5012</v>
       </c>
       <c r="B111" t="str">
-        <v>Lordemil</v>
+        <v>HARRY</v>
       </c>
       <c r="C111" t="str">
-        <v>Tue Oct 08 2024 07:07:11 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 06:42:58</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>1027</v>
+        <v>5012</v>
       </c>
       <c r="B112" t="str">
-        <v>Lordemil</v>
+        <v>HARRY</v>
       </c>
       <c r="C112" t="str">
-        <v>Tue Oct 08 2024 19:50:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:07:07</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>1027</v>
+        <v>5012</v>
       </c>
       <c r="B113" t="str">
-        <v>Lordemil</v>
+        <v>HARRY</v>
       </c>
       <c r="C113" t="str">
-        <v>Wed Oct 09 2024 12:20:46 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 06:58:23</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>1027</v>
+        <v>5012</v>
       </c>
       <c r="B114" t="str">
-        <v>Lordemil</v>
+        <v>HARRY</v>
       </c>
       <c r="C114" t="str">
-        <v>Wed Oct 09 2024 19:07:41 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:00:01</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>1027</v>
+        <v>5012</v>
       </c>
       <c r="B115" t="str">
-        <v>Lordemil</v>
+        <v>HARRY</v>
       </c>
       <c r="C115" t="str">
-        <v>Thu Oct 10 2024 12:45:38 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 06:46:41</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>1027</v>
+        <v>5012</v>
       </c>
       <c r="B116" t="str">
-        <v>Lordemil</v>
+        <v>HARRY</v>
       </c>
       <c r="C116" t="str">
-        <v>Thu Oct 10 2024 14:37:22 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 17:00:51</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>1024</v>
+        <v>5012</v>
       </c>
       <c r="B117" t="str">
-        <v>Jane</v>
+        <v>HARRY</v>
       </c>
       <c r="C117" t="str">
-        <v>Mon Oct 07 2024 08:36:25 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 06:49:17</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>1024</v>
+        <v>5012</v>
       </c>
       <c r="B118" t="str">
-        <v>Jane</v>
+        <v>HARRY</v>
       </c>
       <c r="C118" t="str">
-        <v>Tue Oct 08 2024 07:53:53 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 06:49:19</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>1024</v>
+        <v>2055</v>
       </c>
       <c r="B119" t="str">
-        <v>Jane</v>
+        <v>PAULA</v>
       </c>
       <c r="C119" t="str">
-        <v>Tue Oct 08 2024 15:42:54 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 08:16:46</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>1024</v>
+        <v>2055</v>
       </c>
       <c r="B120" t="str">
-        <v>Jane</v>
+        <v>PAULA</v>
       </c>
       <c r="C120" t="str">
-        <v>Wed Oct 09 2024 07:42:16 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 14:56:56</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>1024</v>
+        <v>2055</v>
       </c>
       <c r="B121" t="str">
-        <v>Jane</v>
+        <v>PAULA</v>
       </c>
       <c r="C121" t="str">
-        <v>Wed Oct 09 2024 15:28:39 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 10:04:53</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>5012</v>
+        <v>2055</v>
       </c>
       <c r="B122" t="str">
-        <v>HARRY</v>
+        <v>PAULA</v>
       </c>
       <c r="C122" t="str">
-        <v>Mon Oct 07 2024 07:02:09 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 16:59:30</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>5012</v>
+        <v>2055</v>
       </c>
       <c r="B123" t="str">
-        <v>HARRY</v>
+        <v>PAULA</v>
       </c>
       <c r="C123" t="str">
-        <v>Mon Oct 07 2024 17:00:48 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:35:03</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>5012</v>
+        <v>2055</v>
       </c>
       <c r="B124" t="str">
-        <v>HARRY</v>
+        <v>PAULA</v>
       </c>
       <c r="C124" t="str">
-        <v>Tue Oct 08 2024 06:50:41 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 11:45:48</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>5012</v>
+        <v>2055</v>
       </c>
       <c r="B125" t="str">
-        <v>HARRY</v>
+        <v>PAULA</v>
       </c>
       <c r="C125" t="str">
-        <v>Tue Oct 08 2024 17:00:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 06:39:03</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>5012</v>
+        <v>1016</v>
       </c>
       <c r="B126" t="str">
-        <v>HARRY</v>
+        <v>BONIFACIO</v>
       </c>
       <c r="C126" t="str">
-        <v>Wed Oct 09 2024 06:42:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 08:56:02</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>5012</v>
+        <v>1016</v>
       </c>
       <c r="B127" t="str">
-        <v>HARRY</v>
+        <v>BONIFACIO</v>
       </c>
       <c r="C127" t="str">
-        <v>Wed Oct 09 2024 17:07:07 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 14:06:32</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>5012</v>
+        <v>1016</v>
       </c>
       <c r="B128" t="str">
-        <v>HARRY</v>
+        <v>BONIFACIO</v>
       </c>
       <c r="C128" t="str">
-        <v>Thu Oct 10 2024 06:58:23 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 08:50:08</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>5012</v>
+        <v>1016</v>
       </c>
       <c r="B129" t="str">
-        <v>HARRY</v>
+        <v>BONIFACIO</v>
       </c>
       <c r="C129" t="str">
-        <v>Thu Oct 10 2024 06:58:26 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:56:04</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>2055</v>
+        <v>1016</v>
       </c>
       <c r="B130" t="str">
-        <v>PAULA</v>
+        <v>BONIFACIO</v>
       </c>
       <c r="C130" t="str">
-        <v>Tue Oct 08 2024 07:11:27 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 09:37:12</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>2055</v>
+        <v>1016</v>
       </c>
       <c r="B131" t="str">
-        <v>PAULA</v>
+        <v>BONIFACIO</v>
       </c>
       <c r="C131" t="str">
-        <v>Tue Oct 08 2024 16:28:00 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 16:33:16</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>2055</v>
+        <v>1021</v>
       </c>
       <c r="B132" t="str">
-        <v>PAULA</v>
+        <v>ERWYN</v>
       </c>
       <c r="C132" t="str">
-        <v>Wed Oct 09 2024 08:16:46 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 12:04:35</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>2055</v>
+        <v>1021</v>
       </c>
       <c r="B133" t="str">
-        <v>PAULA</v>
+        <v>ERWYN</v>
       </c>
       <c r="C133" t="str">
-        <v>Wed Oct 09 2024 14:56:56 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 19:01:08</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>2055</v>
+        <v>1021</v>
       </c>
       <c r="B134" t="str">
-        <v>PAULA</v>
+        <v>ERWYN</v>
       </c>
       <c r="C134" t="str">
-        <v>Thu Oct 10 2024 10:04:53 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 09:59:06</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>2055</v>
+        <v>1021</v>
       </c>
       <c r="B135" t="str">
-        <v>PAULA</v>
+        <v>ERWYN</v>
       </c>
       <c r="C135" t="str">
-        <v>Thu Oct 10 2024 15:17:40 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 18:26:22</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="B136" t="str">
-        <v>BONIFACIO</v>
+        <v>ERWYN</v>
       </c>
       <c r="C136" t="str">
-        <v>Mon Oct 07 2024 08:54:22 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 09:52:34</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="B137" t="str">
-        <v>BONIFACIO</v>
+        <v>ERWYN</v>
       </c>
       <c r="C137" t="str">
-        <v>Mon Oct 07 2024 17:56:56 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 19:02:34</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="B138" t="str">
-        <v>BONIFACIO</v>
+        <v>1007</v>
       </c>
       <c r="C138" t="str">
-        <v>Tue Oct 08 2024 08:51:48 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:56:30</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="B139" t="str">
-        <v>BONIFACIO</v>
+        <v>1007</v>
       </c>
       <c r="C139" t="str">
-        <v>Tue Oct 08 2024 20:30:17 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 13:18:14</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="B140" t="str">
-        <v>BONIFACIO</v>
+        <v>1007</v>
       </c>
       <c r="C140" t="str">
-        <v>Wed Oct 09 2024 08:56:02 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 12:16:16</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="B141" t="str">
-        <v>BONIFACIO</v>
+        <v>1007</v>
       </c>
       <c r="C141" t="str">
-        <v>Wed Oct 09 2024 14:06:32 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 14:31:02</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="B142" t="str">
-        <v>BONIFACIO</v>
+        <v>1007</v>
       </c>
       <c r="C142" t="str">
-        <v>Thu Oct 10 2024 08:50:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 09:18:40</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="B143" t="str">
-        <v>BONIFACIO</v>
+        <v>1007</v>
       </c>
       <c r="C143" t="str">
-        <v>Thu Oct 10 2024 13:14:32 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 12:57:21</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>1021</v>
+        <v>1007</v>
       </c>
       <c r="B144" t="str">
-        <v>ERWYN</v>
+        <v>1007</v>
       </c>
       <c r="C144" t="str">
-        <v>Mon Oct 07 2024 10:03:45 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:54:54</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B145" t="str">
-        <v>ERWYN</v>
+        <v>CESS</v>
       </c>
       <c r="C145" t="str">
-        <v>Mon Oct 07 2024 17:39:57 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 08:01:30</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B146" t="str">
-        <v>ERWYN</v>
+        <v>CESS</v>
       </c>
       <c r="C146" t="str">
-        <v>Tue Oct 08 2024 09:45:18 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 14:17:03</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B147" t="str">
-        <v>ERWYN</v>
+        <v>CESS</v>
       </c>
       <c r="C147" t="str">
-        <v>Tue Oct 08 2024 18:49:31 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:58:08</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B148" t="str">
-        <v>ERWYN</v>
+        <v>CESS</v>
       </c>
       <c r="C148" t="str">
-        <v>Wed Oct 09 2024 12:04:35 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:05:07</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B149" t="str">
-        <v>ERWYN</v>
+        <v>CESS</v>
       </c>
       <c r="C149" t="str">
-        <v>Wed Oct 09 2024 19:01:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 08:06:27</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B150" t="str">
-        <v>ERWYN</v>
+        <v>CESS</v>
       </c>
       <c r="C150" t="str">
-        <v>Thu Oct 10 2024 09:59:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 09:16:16</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B151" t="str">
-        <v>ERWYN</v>
+        <v>CESS</v>
       </c>
       <c r="C151" t="str">
-        <v>Thu Oct 10 2024 11:12:57 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 08:02:56</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="B152" t="str">
-        <v>1007</v>
+        <v>ROXAN</v>
       </c>
       <c r="C152" t="str">
-        <v>Mon Oct 07 2024 07:55:25 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 08:02:59</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="B153" t="str">
-        <v>1007</v>
+        <v>ROXAN</v>
       </c>
       <c r="C153" t="str">
-        <v>Mon Oct 07 2024 16:08:13 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 15:26:12</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="B154" t="str">
-        <v>1007</v>
+        <v>ROXAN</v>
       </c>
       <c r="C154" t="str">
-        <v>Tue Oct 08 2024 08:26:26 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 09:28:26</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="B155" t="str">
-        <v>1007</v>
+        <v>ROXAN</v>
       </c>
       <c r="C155" t="str">
-        <v>Tue Oct 08 2024 11:03:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 11:40:56</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>1007</v>
+        <v>1002</v>
       </c>
       <c r="B156" t="str">
-        <v>1007</v>
+        <v>AFRYL JOY</v>
       </c>
       <c r="C156" t="str">
-        <v>Wed Oct 09 2024 07:56:30 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:41:14</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>1007</v>
+        <v>1002</v>
       </c>
       <c r="B157" t="str">
-        <v>1007</v>
+        <v>AFRYL JOY</v>
       </c>
       <c r="C157" t="str">
-        <v>Wed Oct 09 2024 13:18:14 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 13:01:58</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>1007</v>
+        <v>1002</v>
       </c>
       <c r="B158" t="str">
-        <v>1007</v>
+        <v>AFRYL JOY</v>
       </c>
       <c r="C158" t="str">
-        <v>Thu Oct 10 2024 12:16:16 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 13:09:26</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>1007</v>
+        <v>1002</v>
       </c>
       <c r="B159" t="str">
-        <v>1007</v>
+        <v>AFRYL JOY</v>
       </c>
       <c r="C159" t="str">
-        <v>Thu Oct 10 2024 14:31:02 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 16:04:48</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="B160" t="str">
-        <v>CESS</v>
+        <v>AFRYL JOY</v>
       </c>
       <c r="C160" t="str">
-        <v>Tue Oct 08 2024 07:56:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:36:13</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="B161" t="str">
-        <v>CESS</v>
+        <v>AFRYL JOY</v>
       </c>
       <c r="C161" t="str">
-        <v>Tue Oct 08 2024 11:10:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 12:54:34</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="B162" t="str">
-        <v>CESS</v>
+        <v>AFRYL JOY</v>
       </c>
       <c r="C162" t="str">
-        <v>Wed Oct 09 2024 08:01:30 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 08:39:27</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="B163" t="str">
-        <v>CESS</v>
+        <v>HANNAH</v>
       </c>
       <c r="C163" t="str">
-        <v>Wed Oct 09 2024 14:17:03 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:14:06</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="B164" t="str">
-        <v>CESS</v>
+        <v>HANNAH</v>
       </c>
       <c r="C164" t="str">
-        <v>Thu Oct 10 2024 07:58:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 12:10:48</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="B165" t="str">
-        <v>CESS</v>
+        <v>HANNAH</v>
       </c>
       <c r="C165" t="str">
-        <v>Thu Oct 10 2024 15:01:32 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:13:37</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="B166" t="str">
-        <v>ROXAN</v>
+        <v>HANNAH</v>
       </c>
       <c r="C166" t="str">
-        <v>Mon Oct 07 2024 08:08:36 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 09:23:04</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="B167" t="str">
-        <v>ROXAN</v>
+        <v>HANNAH</v>
       </c>
       <c r="C167" t="str">
-        <v>Mon Oct 07 2024 12:03:34 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:04:49</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="B168" t="str">
-        <v>ROXAN</v>
+        <v>HANNAH</v>
       </c>
       <c r="C168" t="str">
-        <v>Tue Oct 08 2024 10:21:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 13:53:50</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B169" t="str">
-        <v>ROXAN</v>
+        <v>JOHN</v>
       </c>
       <c r="C169" t="str">
-        <v>Wed Oct 09 2024 08:02:59 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:42:23</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B170" t="str">
-        <v>ROXAN</v>
+        <v>JOHN</v>
       </c>
       <c r="C170" t="str">
-        <v>Wed Oct 09 2024 15:26:12 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:42:25</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B171" t="str">
-        <v>ROXAN</v>
+        <v>JOHN</v>
       </c>
       <c r="C171" t="str">
-        <v>Thu Oct 10 2024 09:28:26 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:31:53</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B172" t="str">
-        <v>ROXAN</v>
+        <v>JOHN</v>
       </c>
       <c r="C172" t="str">
-        <v>Thu Oct 10 2024 11:40:56 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:00:48</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="B173" t="str">
-        <v>AFRYL JOY</v>
+        <v>JOHN</v>
       </c>
       <c r="C173" t="str">
-        <v>Mon Oct 07 2024 07:44:11 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 08:02:31</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="B174" t="str">
-        <v>AFRYL JOY</v>
+        <v>JOHN</v>
       </c>
       <c r="C174" t="str">
-        <v>Mon Oct 07 2024 15:07:00 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 17:01:32</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="B175" t="str">
-        <v>AFRYL JOY</v>
+        <v>JOHN</v>
       </c>
       <c r="C175" t="str">
-        <v>Tue Oct 08 2024 07:35:44 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:34:17</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="B176" t="str">
-        <v>AFRYL JOY</v>
+        <v>JOHN</v>
       </c>
       <c r="C176" t="str">
-        <v>Tue Oct 08 2024 12:54:35 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:52:23</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B177" t="str">
-        <v>AFRYL JOY</v>
+        <v>HAYDEE</v>
       </c>
       <c r="C177" t="str">
-        <v>Wed Oct 09 2024 07:41:14 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 11:36:08</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B178" t="str">
-        <v>AFRYL JOY</v>
+        <v>HAYDEE</v>
       </c>
       <c r="C178" t="str">
-        <v>Wed Oct 09 2024 13:01:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:34:52</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B179" t="str">
-        <v>AFRYL JOY</v>
+        <v>HAYDEE</v>
       </c>
       <c r="C179" t="str">
-        <v>Thu Oct 10 2024 13:09:26 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 10:14:17</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>1004</v>
+        <v>1026</v>
       </c>
       <c r="B180" t="str">
-        <v>HANNAH</v>
+        <v>Johnpaul</v>
       </c>
       <c r="C180" t="str">
-        <v>Mon Oct 07 2024 07:49:56 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 10:13:39</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>1004</v>
+        <v>1026</v>
       </c>
       <c r="B181" t="str">
-        <v>HANNAH</v>
+        <v>Johnpaul</v>
       </c>
       <c r="C181" t="str">
-        <v>Mon Oct 07 2024 17:46:55 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 14:52:43</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>1004</v>
+        <v>1026</v>
       </c>
       <c r="B182" t="str">
-        <v>HANNAH</v>
+        <v>Johnpaul</v>
       </c>
       <c r="C182" t="str">
-        <v>Tue Oct 08 2024 13:09:34 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 13:39:34</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>1004</v>
+        <v>1026</v>
       </c>
       <c r="B183" t="str">
-        <v>HANNAH</v>
+        <v>Johnpaul</v>
       </c>
       <c r="C183" t="str">
-        <v>Tue Oct 08 2024 18:14:58 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 15:14:08</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>1004</v>
+        <v>1026</v>
       </c>
       <c r="B184" t="str">
-        <v>HANNAH</v>
+        <v>Johnpaul</v>
       </c>
       <c r="C184" t="str">
-        <v>Wed Oct 09 2024 07:14:06 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 16:48:59</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>1004</v>
+        <v>1026</v>
       </c>
       <c r="B185" t="str">
-        <v>HANNAH</v>
+        <v>Johnpaul</v>
       </c>
       <c r="C185" t="str">
-        <v>Wed Oct 09 2024 12:10:48 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 16:52:31</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>1004</v>
+        <v>1026</v>
       </c>
       <c r="B186" t="str">
-        <v>HANNAH</v>
+        <v>Johnpaul</v>
       </c>
       <c r="C186" t="str">
-        <v>Thu Oct 10 2024 07:13:37 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 06:49:05</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>1004</v>
+        <v>1</v>
       </c>
       <c r="B187" t="str">
-        <v>HANNAH</v>
+        <v>1</v>
       </c>
       <c r="C187" t="str">
-        <v>Thu Oct 10 2024 09:23:04 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 18:41:03</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>1009</v>
+        <v>1</v>
       </c>
       <c r="B188" t="str">
-        <v>JOHN</v>
+        <v>1</v>
       </c>
       <c r="C188" t="str">
-        <v>Mon Oct 07 2024 07:53:45 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 18:41:06</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>1009</v>
+        <v>808</v>
       </c>
       <c r="B189" t="str">
-        <v>JOHN</v>
+        <v>808</v>
       </c>
       <c r="C189" t="str">
-        <v>Mon Oct 07 2024 17:08:51 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 09:40:49</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="B190" t="str">
-        <v>JOHN</v>
+        <v>ANGELICA</v>
       </c>
       <c r="C190" t="str">
-        <v>Tue Oct 08 2024 09:42:02 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 06:58:44</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="B191" t="str">
-        <v>JOHN</v>
+        <v>ANGELICA</v>
       </c>
       <c r="C191" t="str">
-        <v>Tue Oct 08 2024 20:59:03 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:03:04</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="B192" t="str">
-        <v>JOHN</v>
+        <v>ANGELICA</v>
       </c>
       <c r="C192" t="str">
-        <v>Wed Oct 09 2024 07:42:23 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:07:36</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="B193" t="str">
-        <v>JOHN</v>
+        <v>ANGELICA</v>
       </c>
       <c r="C193" t="str">
-        <v>Wed Oct 09 2024 17:42:25 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:02:35</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="B194" t="str">
-        <v>JOHN</v>
+        <v>ANGELICA</v>
       </c>
       <c r="C194" t="str">
-        <v>Thu Oct 10 2024 07:31:53 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:13:06</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>1009</v>
+        <v>1028</v>
       </c>
       <c r="B195" t="str">
-        <v>JOHN</v>
+        <v>ANGELICA</v>
       </c>
       <c r="C195" t="str">
-        <v>Thu Oct 10 2024 14:08:54 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 17:05:31</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>1001</v>
+        <v>1028</v>
       </c>
       <c r="B196" t="str">
-        <v>HAYDEE</v>
+        <v>ANGELICA</v>
       </c>
       <c r="C196" t="str">
-        <v>Mon Oct 07 2024 13:15:52 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-14 07:31:32</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>1001</v>
+        <v>609</v>
       </c>
       <c r="B197" t="str">
-        <v>HAYDEE</v>
+        <v>609</v>
       </c>
       <c r="C197" t="str">
-        <v>Mon Oct 07 2024 18:20:30 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 14:28:16</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>1001</v>
+        <v>609</v>
       </c>
       <c r="B198" t="str">
-        <v>HAYDEE</v>
+        <v>609</v>
       </c>
       <c r="C198" t="str">
-        <v>Tue Oct 08 2024 12:13:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 14:28:18</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>1001</v>
+        <v>3009</v>
       </c>
       <c r="B199" t="str">
-        <v>HAYDEE</v>
+        <v>3009</v>
       </c>
       <c r="C199" t="str">
-        <v>Tue Oct 08 2024 14:39:00 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:58:54</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>1001</v>
+        <v>3009</v>
       </c>
       <c r="B200" t="str">
-        <v>HAYDEE</v>
+        <v>3009</v>
       </c>
       <c r="C200" t="str">
-        <v>Thu Oct 10 2024 11:36:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:47:40</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>1026</v>
+        <v>2009</v>
       </c>
       <c r="B201" t="str">
-        <v>Johnpaul</v>
+        <v>Rachelle</v>
       </c>
       <c r="C201" t="str">
-        <v>Mon Oct 07 2024 08:14:27 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 13:55:04</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>1026</v>
+        <v>12</v>
       </c>
       <c r="B202" t="str">
-        <v>Johnpaul</v>
+        <v>12</v>
       </c>
       <c r="C202" t="str">
-        <v>Mon Oct 07 2024 16:10:22 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 11:38:04</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>1026</v>
+        <v>3</v>
       </c>
       <c r="B203" t="str">
-        <v>Johnpaul</v>
+        <v>3</v>
       </c>
       <c r="C203" t="str">
-        <v>Tue Oct 08 2024 10:56:19 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 15:27:37</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>1026</v>
+        <v>3</v>
       </c>
       <c r="B204" t="str">
-        <v>Johnpaul</v>
+        <v>3</v>
       </c>
       <c r="C204" t="str">
-        <v>Tue Oct 08 2024 16:11:56 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 19:39:30</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>1026</v>
+        <v>3</v>
       </c>
       <c r="B205" t="str">
-        <v>Johnpaul</v>
+        <v>3</v>
       </c>
       <c r="C205" t="str">
-        <v>Wed Oct 09 2024 10:13:39 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 18:03:05</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>1026</v>
+        <v>3</v>
       </c>
       <c r="B206" t="str">
-        <v>Johnpaul</v>
+        <v>3</v>
       </c>
       <c r="C206" t="str">
-        <v>Wed Oct 09 2024 14:52:43 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 21:00:44</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>1026</v>
+        <v>3</v>
       </c>
       <c r="B207" t="str">
-        <v>Johnpaul</v>
+        <v>3</v>
       </c>
       <c r="C207" t="str">
-        <v>Thu Oct 10 2024 13:39:34 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 15:13:22</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>1026</v>
+        <v>3</v>
       </c>
       <c r="B208" t="str">
-        <v>Johnpaul</v>
+        <v>3</v>
       </c>
       <c r="C208" t="str">
-        <v>Thu Oct 10 2024 15:14:08 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 19:59:53</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>808</v>
+        <v>4003</v>
       </c>
       <c r="B209" t="str">
-        <v>808</v>
+        <v>4003</v>
       </c>
       <c r="C209" t="str">
-        <v>Mon Oct 07 2024 10:03:13 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 07:24:51</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>1028</v>
+        <v>5013</v>
       </c>
       <c r="B210" t="str">
-        <v>ANGELICA</v>
+        <v>IRA</v>
       </c>
       <c r="C210" t="str">
-        <v>Mon Oct 07 2024 07:30:34 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 07:28:46</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>1028</v>
+        <v>5013</v>
       </c>
       <c r="B211" t="str">
-        <v>ANGELICA</v>
+        <v>IRA</v>
       </c>
       <c r="C211" t="str">
-        <v>Mon Oct 07 2024 17:11:22 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-09 17:03:31</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>1028</v>
+        <v>5013</v>
       </c>
       <c r="B212" t="str">
-        <v>ANGELICA</v>
+        <v>IRA</v>
       </c>
       <c r="C212" t="str">
-        <v>Tue Oct 08 2024 07:16:05 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 07:41:35</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>1028</v>
+        <v>5013</v>
       </c>
       <c r="B213" t="str">
-        <v>ANGELICA</v>
+        <v>IRA</v>
       </c>
       <c r="C213" t="str">
-        <v>Tue Oct 08 2024 17:03:22 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-10 17:02:12</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>1028</v>
+        <v>5013</v>
       </c>
       <c r="B214" t="str">
-        <v>ANGELICA</v>
+        <v>IRA</v>
       </c>
       <c r="C214" t="str">
-        <v>Wed Oct 09 2024 06:58:44 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 08:10:32</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>1028</v>
+        <v>5013</v>
       </c>
       <c r="B215" t="str">
-        <v>ANGELICA</v>
+        <v>IRA</v>
       </c>
       <c r="C215" t="str">
-        <v>Wed Oct 09 2024 17:03:04 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="str">
-        <v>1028</v>
-      </c>
-      <c r="B216" t="str">
-        <v>ANGELICA</v>
-      </c>
-      <c r="C216" t="str">
-        <v>Thu Oct 10 2024 07:07:36 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="str">
-        <v>1028</v>
-      </c>
-      <c r="B217" t="str">
-        <v>ANGELICA</v>
-      </c>
-      <c r="C217" t="str">
-        <v>Thu Oct 10 2024 11:48:30 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="str">
-        <v>603</v>
-      </c>
-      <c r="B218" t="str">
-        <v>603</v>
-      </c>
-      <c r="C218" t="str">
-        <v>Mon Oct 07 2024 13:33:29 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="str">
-        <v>603</v>
-      </c>
-      <c r="B219" t="str">
-        <v>603</v>
-      </c>
-      <c r="C219" t="str">
-        <v>Mon Oct 07 2024 13:33:41 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="str">
-        <v>604</v>
-      </c>
-      <c r="B220" t="str">
-        <v>604</v>
-      </c>
-      <c r="C220" t="str">
-        <v>Mon Oct 07 2024 13:33:31 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="str">
-        <v>604</v>
-      </c>
-      <c r="B221" t="str">
-        <v>604</v>
-      </c>
-      <c r="C221" t="str">
-        <v>Mon Oct 07 2024 13:33:38 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="str">
-        <v>605</v>
-      </c>
-      <c r="B222" t="str">
-        <v>605</v>
-      </c>
-      <c r="C222" t="str">
-        <v>Mon Oct 07 2024 13:33:33 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="str">
-        <v>605</v>
-      </c>
-      <c r="B223" t="str">
-        <v>605</v>
-      </c>
-      <c r="C223" t="str">
-        <v>Mon Oct 07 2024 13:33:35 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="str">
-        <v>609</v>
-      </c>
-      <c r="B224" t="str">
-        <v>609</v>
-      </c>
-      <c r="C224" t="str">
-        <v>Wed Oct 09 2024 14:28:16 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="str">
-        <v>609</v>
-      </c>
-      <c r="B225" t="str">
-        <v>609</v>
-      </c>
-      <c r="C225" t="str">
-        <v>Wed Oct 09 2024 14:28:18 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="str">
-        <v>3009</v>
-      </c>
-      <c r="B226" t="str">
-        <v>3009</v>
-      </c>
-      <c r="C226" t="str">
-        <v>Wed Oct 09 2024 07:58:54 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="str">
-        <v>10004</v>
-      </c>
-      <c r="B227" t="str">
-        <v>10004</v>
-      </c>
-      <c r="C227" t="str">
-        <v>Mon Oct 07 2024 07:13:55 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="str">
-        <v>10004</v>
-      </c>
-      <c r="B228" t="str">
-        <v>10004</v>
-      </c>
-      <c r="C228" t="str">
-        <v>Mon Oct 07 2024 07:13:57 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="str">
-        <v>10004</v>
-      </c>
-      <c r="B229" t="str">
-        <v>10004</v>
-      </c>
-      <c r="C229" t="str">
-        <v>Tue Oct 08 2024 08:58:49 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="str">
-        <v>2009</v>
-      </c>
-      <c r="B230" t="str">
-        <v>Rachelle</v>
-      </c>
-      <c r="C230" t="str">
-        <v>Tue Oct 08 2024 17:15:29 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="str">
-        <v>12</v>
-      </c>
-      <c r="B231" t="str">
-        <v>12</v>
-      </c>
-      <c r="C231" t="str">
-        <v>Mon Oct 07 2024 09:41:45 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="str">
-        <v>12</v>
-      </c>
-      <c r="B232" t="str">
-        <v>12</v>
-      </c>
-      <c r="C232" t="str">
-        <v>Wed Oct 09 2024 11:38:04 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="str">
-        <v>3</v>
-      </c>
-      <c r="B233" t="str">
-        <v>3</v>
-      </c>
-      <c r="C233" t="str">
-        <v>Mon Oct 07 2024 09:31:40 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="str">
-        <v>3</v>
-      </c>
-      <c r="B234" t="str">
-        <v>3</v>
-      </c>
-      <c r="C234" t="str">
-        <v>Mon Oct 07 2024 18:17:43 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="str">
-        <v>3</v>
-      </c>
-      <c r="B235" t="str">
-        <v>3</v>
-      </c>
-      <c r="C235" t="str">
-        <v>Tue Oct 08 2024 08:03:24 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="str">
-        <v>3</v>
-      </c>
-      <c r="B236" t="str">
-        <v>3</v>
-      </c>
-      <c r="C236" t="str">
-        <v>Tue Oct 08 2024 21:03:04 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="str">
-        <v>3</v>
-      </c>
-      <c r="B237" t="str">
-        <v>3</v>
-      </c>
-      <c r="C237" t="str">
-        <v>Wed Oct 09 2024 15:27:37 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="str">
-        <v>3</v>
-      </c>
-      <c r="B238" t="str">
-        <v>3</v>
-      </c>
-      <c r="C238" t="str">
-        <v>Wed Oct 09 2024 19:39:30 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="str">
-        <v>601</v>
-      </c>
-      <c r="B239" t="str">
-        <v>601</v>
-      </c>
-      <c r="C239" t="str">
-        <v>Mon Oct 07 2024 13:31:13 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="str">
-        <v>601</v>
-      </c>
-      <c r="B240" t="str">
-        <v>601</v>
-      </c>
-      <c r="C240" t="str">
-        <v>Mon Oct 07 2024 13:31:15 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="str">
-        <v>602</v>
-      </c>
-      <c r="B241" t="str">
-        <v>602</v>
-      </c>
-      <c r="C241" t="str">
-        <v>Mon Oct 07 2024 13:33:25 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="str">
-        <v>602</v>
-      </c>
-      <c r="B242" t="str">
-        <v>602</v>
-      </c>
-      <c r="C242" t="str">
-        <v>Mon Oct 07 2024 13:33:43 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="str">
-        <v>5013</v>
-      </c>
-      <c r="B243" t="str">
-        <v>IRA</v>
-      </c>
-      <c r="C243" t="str">
-        <v>Tue Oct 08 2024 08:46:36 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="str">
-        <v>5013</v>
-      </c>
-      <c r="B244" t="str">
-        <v>IRA</v>
-      </c>
-      <c r="C244" t="str">
-        <v>Tue Oct 08 2024 17:04:59 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="str">
-        <v>5013</v>
-      </c>
-      <c r="B245" t="str">
-        <v>IRA</v>
-      </c>
-      <c r="C245" t="str">
-        <v>Wed Oct 09 2024 07:28:46 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="str">
-        <v>5013</v>
-      </c>
-      <c r="B246" t="str">
-        <v>IRA</v>
-      </c>
-      <c r="C246" t="str">
-        <v>Wed Oct 09 2024 17:03:31 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="str">
-        <v>5013</v>
-      </c>
-      <c r="B247" t="str">
-        <v>IRA</v>
-      </c>
-      <c r="C247" t="str">
-        <v>Thu Oct 10 2024 07:41:35 GMT+0800 (Philippine Standard Time)</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="str">
-        <v>5013</v>
-      </c>
-      <c r="B248" t="str">
-        <v>IRA</v>
-      </c>
-      <c r="C248" t="str">
-        <v>Thu Oct 10 2024 13:17:23 GMT+0800 (Philippine Standard Time)</v>
+        <v>2024-10-11 17:06:59</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C248"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C215"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>